<commit_message>
Validation step for the structuring
</commit_message>
<xml_diff>
--- a/data/input/mapping1.xlsx
+++ b/data/input/mapping1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Internship\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Internship\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EC62E6-4008-4FC6-8547-B815E87CF896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43665E28-F1DC-4C4A-9914-5002C3491C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Serie" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="124">
   <si>
     <t>Subject</t>
   </si>
@@ -286,9 +286,6 @@
   </si>
   <si>
     <t>Note</t>
-  </si>
-  <si>
-    <t>Fasciolo S1_SS1_B1_001</t>
   </si>
   <si>
     <t>Immagini S1_SS1_B1_001_01_0001</t>
@@ -827,19 +824,19 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.33203125" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.28515625" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -865,7 +862,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>39</v>
       </c>
@@ -891,24 +888,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>102</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>10</v>
@@ -917,15 +914,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
@@ -934,7 +931,7 @@
         <v>73</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>10</v>
@@ -943,15 +940,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>14</v>
@@ -960,7 +957,7 @@
         <v>74</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>10</v>
@@ -969,7 +966,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>42</v>
       </c>
@@ -991,7 +988,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
@@ -1017,7 +1014,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
@@ -1053,22 +1050,22 @@
   <dimension ref="A1:H10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1094,7 +1091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>49</v>
       </c>
@@ -1120,7 +1117,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>24</v>
       </c>
@@ -1128,7 +1125,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>25</v>
@@ -1137,7 +1134,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>25</v>
@@ -1146,7 +1143,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>49</v>
       </c>
@@ -1163,7 +1160,7 @@
         <v>77</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>28</v>
@@ -1172,41 +1169,41 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>26</v>
@@ -1215,24 +1212,24 @@
         <v>73</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>26</v>
@@ -1241,16 +1238,16 @@
         <v>74</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
@@ -1276,7 +1273,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>49</v>
       </c>
@@ -1302,7 +1299,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>49</v>
       </c>
@@ -1342,18 +1339,18 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="27.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1379,12 +1376,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -1393,10 +1390,10 @@
         <v>34</v>
       </c>
       <c r="E2" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>35</v>
@@ -1405,7 +1402,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>55</v>
       </c>
@@ -1419,7 +1416,7 @@
         <v>34</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>72</v>
@@ -1431,7 +1428,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>55</v>
       </c>
@@ -1457,24 +1454,24 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>35</v>
@@ -1483,15 +1480,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>34</v>
@@ -1500,7 +1497,7 @@
         <v>73</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>35</v>
@@ -1509,15 +1506,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>34</v>
@@ -1526,7 +1523,7 @@
         <v>74</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>35</v>
@@ -1535,24 +1532,24 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>35</v>
@@ -1561,7 +1558,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>55</v>
       </c>
@@ -1587,21 +1584,21 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>120</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
@@ -1611,21 +1608,21 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>55</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
@@ -1645,21 +1642,21 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.33203125" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="4" max="4" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20" customWidth="1"/>
+    <col min="7" max="8" width="23.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1685,7 +1682,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>67</v>
       </c>
@@ -1708,27 +1705,27 @@
         <v>63</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>63</v>
@@ -1737,15 +1734,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>62</v>
@@ -1754,7 +1751,7 @@
         <v>73</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>63</v>
@@ -1763,24 +1760,24 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>62</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>63</v>
@@ -1789,15 +1786,15 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="4" t="s">
         <v>106</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>107</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>62</v>
@@ -1806,7 +1803,7 @@
         <v>74</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>63</v>
@@ -1815,7 +1812,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>66</v>
       </c>
@@ -1838,10 +1835,10 @@
         <v>63</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.3">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>79</v>
       </c>
@@ -1867,7 +1864,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>66</v>
       </c>
@@ -1881,7 +1878,7 @@
         <v>62</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>71</v>
@@ -1890,10 +1887,10 @@
         <v>63</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
@@ -1907,7 +1904,7 @@
         <v>62</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>59</v>
@@ -1917,7 +1914,7 @@
       </c>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>66</v>
       </c>
@@ -1943,7 +1940,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>55</v>
       </c>
@@ -1960,7 +1957,7 @@
         <v>78</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>35</v>
@@ -1969,12 +1966,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>66</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>7</v>
@@ -1983,10 +1980,10 @@
         <v>62</v>
       </c>
       <c r="E13" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="F13" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>117</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>63</v>
@@ -2004,22 +2001,22 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -2045,127 +2042,71 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>10</v>
-      </c>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
       <c r="H2" s="4"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>28</v>
-      </c>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="4"/>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
       <c r="H3" s="4"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>31</v>
-      </c>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
       <c r="H4" s="4"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H5" s="4"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>85</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>87</v>
-      </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>39</v>
       </c>
@@ -2179,7 +2120,7 @@
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>72</v>
@@ -2191,7 +2132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>49</v>
       </c>
@@ -2205,7 +2146,7 @@
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>72</v>
@@ -2217,7 +2158,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>54</v>
       </c>
@@ -2231,7 +2172,7 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>72</v>
@@ -2243,7 +2184,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>55</v>
       </c>
@@ -2257,7 +2198,7 @@
         <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F10" s="4" t="s">
         <v>72</v>
@@ -2269,7 +2210,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>67</v>
       </c>
@@ -2283,7 +2224,7 @@
         <v>62</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>72</v>
@@ -2295,44 +2236,44 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F12" s="4" t="s">
         <v>72</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>77</v>
@@ -2341,13 +2282,13 @@
         <v>15</v>
       </c>
       <c r="G13" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="H13" s="4" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>67</v>
       </c>
@@ -2355,7 +2296,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D14" s="4" t="s">
         <v>62</v>
@@ -2364,16 +2305,16 @@
         <v>6</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>63</v>
       </c>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>27</v>
@@ -2382,7 +2323,7 @@
         <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>76</v>
@@ -2391,13 +2332,13 @@
         <v>75</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="8"/>

</xml_diff>

<commit_message>
Updated script handling of busta level
Updated direct inclusion relationships with busta and UML diagrams
</commit_message>
<xml_diff>
--- a/data/input/mapping1.xlsx
+++ b/data/input/mapping1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Documents\GitHub\Internship\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43665E28-F1DC-4C4A-9914-5002C3491C05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6745AD05-6C90-4284-B8BF-B08A0C7AAA6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Serie" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="122">
   <si>
     <t>Subject</t>
   </si>
@@ -196,12 +196,6 @@
   </si>
   <si>
     <t>Corrispondenza di Giuseppe Albini con diversi [...]</t>
-  </si>
-  <si>
-    <t>Buste 1-11; busta 13, fascc. 1, 2, 4</t>
-  </si>
-  <si>
-    <t>Notes</t>
   </si>
   <si>
     <t>Busta S1_SS1_B1</t>
@@ -876,7 +870,7 @@
         <v>14</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>15</v>
@@ -893,19 +887,19 @@
         <v>39</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>10</v>
@@ -919,19 +913,19 @@
         <v>39</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>10</v>
@@ -945,19 +939,19 @@
         <v>39</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>10</v>
@@ -1049,8 +1043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95813D3A-72E7-4BB6-8FB9-93240D7FEB11}">
   <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1105,10 +1099,10 @@
         <v>26</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>28</v>
@@ -1125,7 +1119,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>25</v>
@@ -1134,7 +1128,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>25</v>
@@ -1157,10 +1151,10 @@
         <v>26</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>28</v>
@@ -1174,25 +1168,25 @@
         <v>49</v>
       </c>
       <c r="B5" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="4" t="s">
         <v>101</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>103</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1200,25 +1194,25 @@
         <v>49</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1226,25 +1220,25 @@
         <v>49</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>28</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1300,30 +1294,14 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G10" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="4" t="s">
-        <v>53</v>
-      </c>
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -1378,10 +1356,10 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>7</v>
@@ -1390,10 +1368,10 @@
         <v>34</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>35</v>
@@ -1404,7 +1382,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>29</v>
@@ -1416,10 +1394,10 @@
         <v>34</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>35</v>
@@ -1430,7 +1408,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>13</v>
@@ -1442,7 +1420,7 @@
         <v>34</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F4" s="4" t="s">
         <v>15</v>
@@ -1456,22 +1434,22 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>35</v>
@@ -1482,22 +1460,22 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>35</v>
@@ -1508,22 +1486,22 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>35</v>
@@ -1534,22 +1512,22 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>35</v>
@@ -1560,13 +1538,13 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>34</v>
@@ -1586,19 +1564,19 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D10" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F10" s="4"/>
       <c r="G10" s="4" t="s">
@@ -1610,19 +1588,19 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>34</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F11" s="4"/>
       <c r="G11" s="4" t="s">
@@ -1684,172 +1662,172 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G3" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G4" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H4" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="C5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="F5" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H5" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G6" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H6" s="4" t="s">
         <v>63</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>44</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>46</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>20</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>48</v>
@@ -1858,65 +1836,65 @@
         <v>15</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="G9" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>62</v>
-      </c>
       <c r="E10" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>27</v>
@@ -1925,16 +1903,16 @@
         <v>7</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>35</v>
@@ -1942,7 +1920,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B12" s="7" t="s">
         <v>18</v>
@@ -1954,39 +1932,39 @@
         <v>34</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G12" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H13" s="4"/>
     </row>
@@ -2000,7 +1978,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{750A8FC3-B2D9-4857-BDBF-97A1C08E4AF5}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2084,25 +2062,25 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H6" s="4"/>
     </row>
@@ -2120,10 +2098,10 @@
         <v>14</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>10</v>
@@ -2146,10 +2124,10 @@
         <v>26</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>28</v>
@@ -2160,7 +2138,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -2172,10 +2150,10 @@
         <v>32</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>31</v>
@@ -2186,7 +2164,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>29</v>
@@ -2198,10 +2176,10 @@
         <v>34</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>35</v>
@@ -2212,109 +2190,109 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C11" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>63</v>
-      </c>
       <c r="H11" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>29</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D12" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E12" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="H12" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>84</v>
-      </c>
       <c r="E13" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>6</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>27</v>
@@ -2323,19 +2301,19 @@
         <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="E15" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>86</v>
-      </c>
       <c r="H15" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>